<commit_message>
BugFixs RoomType and Select Hotel
</commit_message>
<xml_diff>
--- a/doc/documentation/Roots.xlsx
+++ b/doc/documentation/Roots.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WallQ-\Documents\GitHub\PWA\doc\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\PWA\doc\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03B5D42-3D8E-48CD-9210-9BAFDB1F043D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A161D82B-7B5D-4479-8DE3-BEB319A32A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4268568D-A048-4D06-9752-F2A98D35CC0F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4268568D-A048-4D06-9752-F2A98D35CC0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="104">
   <si>
     <t>Requisição</t>
   </si>
@@ -331,6 +331,21 @@
   </si>
   <si>
     <t>Obter reserva do utilizador</t>
+  </si>
+  <si>
+    <t>/signed</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>/:userID</t>
+  </si>
+  <si>
+    <t>/workingon</t>
+  </si>
+  <si>
+    <t>Obter os Hotel com permissão</t>
   </si>
 </sst>
 </file>
@@ -338,7 +353,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -406,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,6 +447,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -535,13 +556,13 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -594,6 +615,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -615,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,6 +649,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -946,13 +973,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76465699-1A4C-4BD8-B810-481E3C1F192C}">
-  <dimension ref="B2:Z57"/>
+  <dimension ref="B2:Z59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10:F10"/>
+      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,23 +1002,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="L2" s="23" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="L2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="26"/>
       <c r="Q2" s="16"/>
       <c r="R2" s="17"/>
       <c r="S2" s="17"/>
@@ -1007,12 +1034,12 @@
       <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="18" t="s">
         <v>2</v>
       </c>
@@ -1050,7 +1077,7 @@
       <c r="Z3" s="17"/>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -1059,10 +1086,10 @@
       <c r="D4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="29"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11" t="s">
         <v>9</v>
@@ -1101,17 +1128,17 @@
       <c r="Z4" s="17"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12" t="s">
         <v>12</v>
@@ -1144,7 +1171,7 @@
       <c r="Z5" s="17"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="11" t="s">
         <v>6</v>
       </c>
@@ -1195,29 +1222,27 @@
       <c r="Z6" s="17"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11" t="s">
-        <v>95</v>
+      <c r="E7" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="J7" s="4"/>
       <c r="K7" s="3"/>
       <c r="L7" s="4" t="s">
         <v>10</v>
@@ -1228,12 +1253,8 @@
       <c r="N7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="10"/>
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
       <c r="S7" s="17"/>
@@ -1246,22 +1267,22 @@
       <c r="Z7" s="17"/>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7" t="s">
-        <v>15</v>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>10</v>
@@ -1276,8 +1297,12 @@
       <c r="M8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="N8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="P8" s="10" t="s">
         <v>91</v>
       </c>
@@ -1293,22 +1318,22 @@
       <c r="Z8" s="17"/>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="C9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8" t="s">
-        <v>17</v>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>10</v>
@@ -1320,11 +1345,11 @@
       <c r="L9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="N9" s="4"/>
-      <c r="O9" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="O9" s="4"/>
       <c r="P9" s="10" t="s">
         <v>91</v>
       </c>
@@ -1340,22 +1365,22 @@
       <c r="Z9" s="17"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11" t="s">
-        <v>21</v>
+      <c r="F10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>10</v>
@@ -1367,13 +1392,11 @@
       <c r="L10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="P10" s="10" t="s">
         <v>91</v>
       </c>
@@ -1389,7 +1412,7 @@
       <c r="Z10" s="17"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="11" t="s">
         <v>6</v>
       </c>
@@ -1400,11 +1423,11 @@
         <v>13</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>10</v>
@@ -1422,9 +1445,7 @@
       <c r="N11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="O11" s="4"/>
       <c r="P11" s="10" t="s">
         <v>91</v>
       </c>
@@ -1440,7 +1461,7 @@
       <c r="Z11" s="17"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B12" s="26"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="11" t="s">
         <v>6</v>
       </c>
@@ -1451,11 +1472,11 @@
         <v>13</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>10</v>
@@ -1473,7 +1494,9 @@
       <c r="N12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O12" s="4"/>
+      <c r="O12" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="P12" s="10" t="s">
         <v>91</v>
       </c>
@@ -1489,7 +1512,7 @@
       <c r="Z12" s="17"/>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="11" t="s">
         <v>6</v>
       </c>
@@ -1500,11 +1523,11 @@
         <v>13</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>10</v>
@@ -1538,6 +1561,43 @@
       <c r="Z13" s="17"/>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="27"/>
+      <c r="C14" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
       <c r="S14" s="17"/>
@@ -1549,44 +1609,7 @@
       <c r="Y14" s="17"/>
       <c r="Z14" s="17"/>
     </row>
-    <row r="15" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O15" s="4"/>
-      <c r="P15" s="10" t="s">
-        <v>91</v>
-      </c>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
       <c r="S15" s="17"/>
@@ -1598,21 +1621,23 @@
       <c r="Y15" s="17"/>
       <c r="Z15" s="17"/>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="C16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="12" t="s">
+    <row r="16" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12" t="s">
-        <v>25</v>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>10</v>
@@ -1627,34 +1652,44 @@
       <c r="M16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N16" s="4"/>
+      <c r="N16" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="O16" s="4"/>
       <c r="P16" s="10" t="s">
         <v>91</v>
       </c>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
-      <c r="C17" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="11" t="s">
+      <c r="B17" s="27"/>
+      <c r="C17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="11" t="s">
+      <c r="E17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11" t="s">
-        <v>26</v>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K17" s="3"/>
@@ -1664,36 +1699,34 @@
       <c r="M17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N17" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
-      <c r="C18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7" t="s">
-        <v>27</v>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="14" t="s">
         <v>10</v>
       </c>
       <c r="K18" s="3"/>
@@ -1703,29 +1736,31 @@
       <c r="M18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N18" s="4"/>
+      <c r="N18" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="O18" s="4"/>
       <c r="P18" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
-      <c r="C19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="B19" s="27"/>
+      <c r="C19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8" t="s">
-        <v>28</v>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>10</v>
@@ -1747,22 +1782,22 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
-      <c r="C20" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11" t="s">
-        <v>62</v>
+      <c r="F20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>10</v>
@@ -1770,77 +1805,75 @@
       <c r="J20" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="K20" s="3"/>
       <c r="L20" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N20" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="S20" s="15"/>
-    </row>
-    <row r="22" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="27"/>
+      <c r="C21" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O21" s="4"/>
+      <c r="P21" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="S21" s="15"/>
+    </row>
+    <row r="23" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5" t="s">
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P22" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="26"/>
-      <c r="C23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>10</v>
@@ -1855,66 +1888,66 @@
       <c r="M23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
+      <c r="N23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="P23" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="26"/>
-      <c r="C24" s="5" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="27"/>
+      <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5" t="s">
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K24" s="1"/>
-      <c r="L24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P24" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="26"/>
-      <c r="C25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>10</v>
@@ -1929,27 +1962,31 @@
       <c r="M25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
+      <c r="N25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="P25" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="26"/>
-      <c r="C26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="8" t="s">
+      <c r="B26" s="27"/>
+      <c r="C26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8" t="s">
-        <v>33</v>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>10</v>
@@ -1970,23 +2007,21 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="26"/>
-      <c r="C27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="5" t="s">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="27"/>
+      <c r="C27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5" t="s">
-        <v>63</v>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>10</v>
@@ -1994,22 +2029,21 @@
       <c r="J27" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="K27" s="1"/>
       <c r="L27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O27" s="13"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
       <c r="P27" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="28" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="26"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="5" t="s">
         <v>6</v>
       </c>
@@ -2020,11 +2054,11 @@
         <v>13</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>10</v>
@@ -2041,13 +2075,13 @@
       <c r="N28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O28" s="4"/>
+      <c r="O28" s="13"/>
       <c r="P28" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="29" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="26"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="5" t="s">
         <v>6</v>
       </c>
@@ -2058,11 +2092,11 @@
         <v>13</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>10</v>
@@ -2084,61 +2118,62 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="27" t="s">
+    <row r="30" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="27"/>
+      <c r="C30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O30" s="4"/>
+      <c r="P30" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5" t="s">
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O31" s="4"/>
-      <c r="P31" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="27"/>
-      <c r="C32" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>10</v>
@@ -2156,30 +2191,26 @@
       <c r="N32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O32" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="O32" s="4"/>
       <c r="P32" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="27"/>
-      <c r="C33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="B33" s="28"/>
+      <c r="C33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="E33" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5" t="s">
-        <v>38</v>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>10</v>
@@ -2205,22 +2236,22 @@
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="27"/>
-      <c r="C34" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="7" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7" t="s">
-        <v>39</v>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>10</v>
@@ -2238,28 +2269,30 @@
       <c r="N34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O34" s="4"/>
+      <c r="O34" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="P34" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="27"/>
-      <c r="C35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="8" t="s">
+      <c r="B35" s="28"/>
+      <c r="C35" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8" t="s">
-        <v>40</v>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>10</v>
@@ -2283,97 +2316,101 @@
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="27"/>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="28"/>
+      <c r="C36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" s="3"/>
+      <c r="L36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O36" s="4"/>
+      <c r="P36" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="28"/>
+      <c r="C37" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6" t="s">
+      <c r="G37" s="6"/>
+      <c r="H37" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P36" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="27" t="s">
+      <c r="I37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P37" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5" t="s">
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K38" s="3"/>
-      <c r="L38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="27"/>
-      <c r="C39" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>10</v>
@@ -2395,22 +2432,20 @@
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="27"/>
-      <c r="C40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="B40" s="28"/>
+      <c r="C40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="5" t="s">
+      <c r="E40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5" t="s">
-        <v>45</v>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>10</v>
@@ -2425,31 +2460,29 @@
       <c r="M40" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N40" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="27"/>
-      <c r="C41" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="7" t="s">
+      <c r="B41" s="28"/>
+      <c r="C41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7" t="s">
-        <v>87</v>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>10</v>
@@ -2464,29 +2497,31 @@
       <c r="M41" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N41" s="4"/>
+      <c r="N41" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="O41" s="4"/>
       <c r="P41" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="27"/>
-      <c r="C42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="8" t="s">
+      <c r="B42" s="28"/>
+      <c r="C42" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8" t="s">
-        <v>46</v>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>10</v>
@@ -2507,48 +2542,47 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="26" t="s">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="28"/>
+      <c r="C43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K43" s="3"/>
+      <c r="L43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P44" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="26"/>
       <c r="C45" s="6" t="s">
         <v>11</v>
       </c>
@@ -2556,217 +2590,229 @@
         <v>66</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="27"/>
+      <c r="C46" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P45" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="26"/>
-      <c r="C46" s="5" t="s">
+      <c r="I46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P46" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="27"/>
+      <c r="C47" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D47" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E47" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P47" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="27"/>
+      <c r="C48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5" t="s">
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P46" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="26"/>
-      <c r="C47" s="6" t="s">
+      <c r="I48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P48" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B49" s="27"/>
+      <c r="C49" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E49" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6" t="s">
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="I47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P47" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="26"/>
-      <c r="C48" s="6" t="s">
+      <c r="I49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P49" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B50" s="27"/>
+      <c r="C50" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E50" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="12" t="s">
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="I48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P48" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="20" t="s">
+      <c r="I50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P50" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" s="19"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="21"/>
-      <c r="C51" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-      <c r="P51" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B52" s="21"/>
       <c r="C52" s="11" t="s">
         <v>6</v>
       </c>
@@ -2774,14 +2820,12 @@
         <v>78</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>80</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F52" s="19"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I52" s="4" t="s">
         <v>10</v>
@@ -2792,32 +2836,28 @@
       <c r="L52" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M52" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N52" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
       <c r="O52" s="4"/>
       <c r="P52" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="21"/>
-      <c r="C53" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="7" t="s">
+      <c r="B53" s="22"/>
+      <c r="C53" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E53" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7" t="s">
-        <v>93</v>
+      <c r="E53" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12" t="s">
+        <v>84</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>10</v>
@@ -2828,21 +2868,15 @@
       <c r="L53" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M53" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N53" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O53" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
       <c r="P53" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="21"/>
+      <c r="B54" s="22"/>
       <c r="C54" s="11" t="s">
         <v>6</v>
       </c>
@@ -2853,11 +2887,11 @@
         <v>79</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>10</v>
@@ -2874,15 +2908,13 @@
       <c r="N54" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O54" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="O54" s="4"/>
       <c r="P54" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="21"/>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B55" s="22"/>
       <c r="C55" s="7" t="s">
         <v>14</v>
       </c>
@@ -2890,14 +2922,12 @@
         <v>78</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>82</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="F55" s="7"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>10</v>
@@ -2921,23 +2951,23 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="21"/>
-      <c r="C56" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D56" s="8" t="s">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B56" s="22"/>
+      <c r="C56" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="F56" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8" t="s">
-        <v>89</v>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>10</v>
@@ -2963,58 +2993,138 @@
     </row>
     <row r="57" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="22"/>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P57" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="22"/>
+      <c r="C58" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P58" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="23"/>
+      <c r="C59" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="D59" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="E59" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="F59" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11" t="s">
+      <c r="G59" s="11"/>
+      <c r="H59" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P57" s="10" t="s">
+      <c r="I59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P59" s="10" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B50:B57"/>
+    <mergeCell ref="B52:B59"/>
     <mergeCell ref="L2:P2"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="B39:B43"/>
     <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="B4:B14"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B32:B37"/>
     <mergeCell ref="C2:J2"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B23:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new pages, api fixes
</commit_message>
<xml_diff>
--- a/doc/documentation/Roots.xlsx
+++ b/doc/documentation/Roots.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\PWA\doc\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WallQ-\Documents\GitHub\PWA\doc\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A161D82B-7B5D-4479-8DE3-BEB319A32A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97AB1ED-95BE-4E65-B8AA-056A485238B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4268568D-A048-4D06-9752-F2A98D35CC0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4268568D-A048-4D06-9752-F2A98D35CC0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="104">
   <si>
     <t>Requisição</t>
   </si>
@@ -353,7 +353,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -556,7 +556,7 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -618,6 +618,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -639,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -649,9 +652,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,7 +979,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,23 +1002,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="L2" s="24" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="L2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="16"/>
       <c r="R2" s="17"/>
       <c r="S2" s="17"/>
@@ -1034,12 +1034,12 @@
       <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
       <c r="H3" s="18" t="s">
         <v>2</v>
       </c>
@@ -1077,7 +1077,7 @@
       <c r="Z3" s="17"/>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -1086,10 +1086,10 @@
       <c r="D4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="30"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11" t="s">
         <v>9</v>
@@ -1128,17 +1128,17 @@
       <c r="Z4" s="17"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="31"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12" t="s">
         <v>12</v>
@@ -1171,7 +1171,7 @@
       <c r="Z5" s="17"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="27"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="11" t="s">
         <v>6</v>
       </c>
@@ -1222,7 +1222,7 @@
       <c r="Z6" s="17"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="20" t="s">
         <v>6</v>
       </c>
@@ -1267,7 +1267,7 @@
       <c r="Z7" s="17"/>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="27"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="11" t="s">
         <v>6</v>
       </c>
@@ -1318,7 +1318,7 @@
       <c r="Z8" s="17"/>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1365,7 +1365,7 @@
       <c r="Z9" s="17"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
@@ -1394,9 +1394,7 @@
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="O10" s="4"/>
       <c r="P10" s="10" t="s">
         <v>91</v>
       </c>
@@ -1412,7 +1410,7 @@
       <c r="Z10" s="17"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="11" t="s">
         <v>6</v>
       </c>
@@ -1461,7 +1459,7 @@
       <c r="Z11" s="17"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="11" t="s">
         <v>6</v>
       </c>
@@ -1512,7 +1510,7 @@
       <c r="Z12" s="17"/>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B13" s="27"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="11" t="s">
         <v>6</v>
       </c>
@@ -1561,7 +1559,7 @@
       <c r="Z13" s="17"/>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="11" t="s">
         <v>6</v>
       </c>
@@ -1622,7 +1620,7 @@
       <c r="Z15" s="17"/>
     </row>
     <row r="16" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -1671,7 +1669,7 @@
       <c r="Z16" s="17"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="27"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="12" t="s">
         <v>11</v>
       </c>
@@ -1706,7 +1704,7 @@
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="27"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="11" t="s">
         <v>6</v>
       </c>
@@ -1745,7 +1743,7 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="7" t="s">
         <v>14</v>
       </c>
@@ -1782,7 +1780,7 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="8" t="s">
         <v>16</v>
       </c>
@@ -1819,7 +1817,7 @@
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="27"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="11" t="s">
         <v>6</v>
       </c>
@@ -1858,7 +1856,7 @@
       <c r="S21" s="15"/>
     </row>
     <row r="23" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="28" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -1899,7 +1897,7 @@
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="27"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="6" t="s">
         <v>11</v>
       </c>
@@ -1934,7 +1932,7 @@
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
@@ -1973,7 +1971,7 @@
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="27"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="7" t="s">
         <v>14</v>
       </c>
@@ -2008,7 +2006,7 @@
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="8" t="s">
         <v>16</v>
       </c>
@@ -2043,7 +2041,7 @@
       </c>
     </row>
     <row r="28" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="27"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="5" t="s">
         <v>6</v>
       </c>
@@ -2081,7 +2079,7 @@
       </c>
     </row>
     <row r="29" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="27"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="5" t="s">
         <v>6</v>
       </c>
@@ -2119,7 +2117,7 @@
       </c>
     </row>
     <row r="30" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="27"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="5" t="s">
         <v>6</v>
       </c>
@@ -2158,7 +2156,7 @@
     </row>
     <row r="31" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="29" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="5" t="s">
@@ -2197,7 +2195,7 @@
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="28"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="6" t="s">
         <v>11</v>
       </c>
@@ -2236,7 +2234,7 @@
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="28"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
@@ -2277,7 +2275,7 @@
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="28"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="7" t="s">
         <v>14</v>
       </c>
@@ -2316,7 +2314,7 @@
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="28"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="8" t="s">
         <v>16</v>
       </c>
@@ -2355,7 +2353,7 @@
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="28"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="6" t="s">
         <v>11</v>
       </c>
@@ -2395,7 +2393,7 @@
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="29" t="s">
         <v>41</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2432,7 +2430,7 @@
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="28"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="6" t="s">
         <v>11</v>
       </c>
@@ -2467,7 +2465,7 @@
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="28"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="5" t="s">
         <v>6</v>
       </c>
@@ -2506,7 +2504,7 @@
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="28"/>
+      <c r="B42" s="29"/>
       <c r="C42" s="7" t="s">
         <v>14</v>
       </c>
@@ -2543,7 +2541,7 @@
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="28"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="8" t="s">
         <v>16</v>
       </c>
@@ -2580,7 +2578,7 @@
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="28" t="s">
         <v>76</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -2620,7 +2618,7 @@
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="27"/>
+      <c r="B46" s="28"/>
       <c r="C46" s="6" t="s">
         <v>11</v>
       </c>
@@ -2658,19 +2656,19 @@
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="27"/>
-      <c r="C47" s="32" t="s">
+      <c r="B47" s="28"/>
+      <c r="C47" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="32" t="s">
+      <c r="E47" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32" t="s">
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21" t="s">
         <v>100</v>
       </c>
       <c r="I47" s="4" t="s">
@@ -2696,7 +2694,7 @@
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="27"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="5" t="s">
         <v>6</v>
       </c>
@@ -2734,7 +2732,7 @@
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="27"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="6" t="s">
         <v>11</v>
       </c>
@@ -2772,7 +2770,7 @@
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B50" s="27"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="6" t="s">
         <v>11</v>
       </c>
@@ -2810,7 +2808,7 @@
       </c>
     </row>
     <row r="52" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="22" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11" t="s">
@@ -2844,7 +2842,7 @@
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="22"/>
+      <c r="B53" s="23"/>
       <c r="C53" s="12" t="s">
         <v>11</v>
       </c>
@@ -2876,7 +2874,7 @@
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="22"/>
+      <c r="B54" s="23"/>
       <c r="C54" s="11" t="s">
         <v>6</v>
       </c>
@@ -2914,7 +2912,7 @@
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="22"/>
+      <c r="B55" s="23"/>
       <c r="C55" s="7" t="s">
         <v>14</v>
       </c>
@@ -2952,7 +2950,7 @@
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B56" s="22"/>
+      <c r="B56" s="23"/>
       <c r="C56" s="11" t="s">
         <v>6</v>
       </c>
@@ -2992,7 +2990,7 @@
       </c>
     </row>
     <row r="57" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="22"/>
+      <c r="B57" s="23"/>
       <c r="C57" s="7" t="s">
         <v>14</v>
       </c>
@@ -3032,7 +3030,7 @@
       </c>
     </row>
     <row r="58" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="22"/>
+      <c r="B58" s="23"/>
       <c r="C58" s="8" t="s">
         <v>16</v>
       </c>
@@ -3072,7 +3070,7 @@
       </c>
     </row>
     <row r="59" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="23"/>
+      <c r="B59" s="24"/>
       <c r="C59" s="11" t="s">
         <v>6</v>
       </c>

</xml_diff>